<commit_message>
Adjustments to create compatibility with the Delft-FIAT executable.
</commit_message>
<xml_diff>
--- a/examples/results/fiat_test/fiat_configuration.xlsx
+++ b/examples/results/fiat_test/fiat_configuration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11325" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" state="visible" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -542,16 +542,25 @@
     <col width="18.28515625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
     <col width="18.28515625" customWidth="1" style="2" min="3" max="3"/>
     <col hidden="1" width="11.7109375" customWidth="1" style="2" min="4" max="4"/>
-    <col hidden="1" width="13.7109375" customWidth="1" style="2" min="5" max="5"/>
+    <col hidden="1" width="9.140625" customWidth="1" style="2" min="5" max="5"/>
     <col width="15.28515625" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
-    <col hidden="1" width="11.28515625" customWidth="1" style="2" min="7" max="7"/>
+    <col hidden="1" width="9.140625" customWidth="1" style="2" min="7" max="7"/>
     <col width="9.5703125" customWidth="1" style="2" min="8" max="8"/>
     <col width="19.28515625" customWidth="1" style="2" min="9" max="9"/>
     <col width="34.5703125" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
+      <c r="A1" s="16" t="inlineStr">
+        <is>
+          <t>Country Tag</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
       <c r="C1" s="16" t="inlineStr">
         <is>
           <t>INC File Filepath</t>
@@ -588,14 +597,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="inlineStr">
-        <is>
-          <t>Country Tag</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Hazard Type</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C3" s="16" t="inlineStr">
@@ -644,14 +653,14 @@
       <c r="K4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Hazard Type</t>
+      <c r="A5" s="16" t="inlineStr">
+        <is>
+          <t>Unit</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>flooding</t>
+          <t>ft</t>
         </is>
       </c>
       <c r="C5" s="16" t="inlineStr">
@@ -686,7 +695,11 @@
           <t>Maximum Damage</t>
         </is>
       </c>
-      <c r="D6" s="1" t="n"/>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>BU</t>
+        </is>
+      </c>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
@@ -727,6 +740,9 @@
       </c>
       <c r="C7" t="n">
         <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>

</xml_diff>